<commit_message>
Serial bridge ok, animation plays, Mp3 is meh
</commit_message>
<xml_diff>
--- a/pinout.xlsx
+++ b/pinout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\repos\br3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C24741-9CA7-4796-8044-92BC9DF17797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36D99482-5BA8-4F63-8543-EFA5FE0B6C9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{8220847F-6506-48F0-B82A-383ABFBD9DB4}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="3960" windowWidth="18195" windowHeight="10110" activeTab="1" xr2:uid="{8220847F-6506-48F0-B82A-383ABFBD9DB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -907,7 +907,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1191,7 +1191,7 @@
         <v>8</v>
       </c>
       <c r="I13" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="J13" t="s">
         <v>52</v>

</xml_diff>